<commit_message>
Testing MSO playbook completed
</commit_message>
<xml_diff>
--- a/all-mso-config.xlsx
+++ b/all-mso-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="mso-site" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="117">
   <si>
     <t xml:space="preserve">site</t>
   </si>
   <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
     <t xml:space="preserve">siteid</t>
   </si>
   <si>
@@ -57,13 +54,13 @@
     <t xml:space="preserve">site1</t>
   </si>
   <si>
-    <t xml:space="preserve">Site 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">10.10.20.14</t>
   </si>
   <si>
-    <t xml:space="preserve">#</t>
+    <t xml:space="preserve">10.10.20.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.10.20.16</t>
   </si>
   <si>
     <t xml:space="preserve">present</t>
@@ -186,10 +183,10 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">flood</t>
@@ -222,6 +219,12 @@
     <t xml:space="preserve">172.17.3.1/24</t>
   </si>
   <si>
+    <t xml:space="preserve">bd-web4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
     <t xml:space="preserve">l3out-site1-ext-epg</t>
   </si>
   <si>
@@ -270,6 +273,9 @@
     <t xml:space="preserve">ip</t>
   </si>
   <si>
+    <t xml:space="preserve">unspecified</t>
+  </si>
+  <si>
     <t xml:space="preserve">udp-tcp-53</t>
   </si>
   <si>
@@ -318,15 +324,15 @@
     <t xml:space="preserve">permit-dns</t>
   </si>
   <si>
-    <t xml:space="preserve">one-way</t>
-  </si>
-  <si>
     <t xml:space="preserve">log</t>
   </si>
   <si>
     <t xml:space="preserve">permit-https</t>
   </si>
   <si>
+    <t xml:space="preserve">multisite</t>
+  </si>
+  <si>
     <t xml:space="preserve">epg</t>
   </si>
   <si>
@@ -336,42 +342,15 @@
     <t xml:space="preserve">epg1</t>
   </si>
   <si>
-    <t xml:space="preserve">bd1</t>
-  </si>
-  <si>
     <t xml:space="preserve">epg2</t>
   </si>
   <si>
-    <t xml:space="preserve">bd2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">custumer1</t>
-  </si>
-  <si>
     <t xml:space="preserve">epg3</t>
   </si>
   <si>
-    <t xml:space="preserve">bd3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">custumer2</t>
-  </si>
-  <si>
     <t xml:space="preserve">epg4</t>
   </si>
   <si>
-    <t xml:space="preserve">bd4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">custumer3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epg5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bd5</t>
-  </si>
-  <si>
     <t xml:space="preserve">domaintype</t>
   </si>
   <si>
@@ -384,10 +363,10 @@
     <t xml:space="preserve">resolutionimmediacy</t>
   </si>
   <si>
-    <t xml:space="preserve">vmmDomain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vmm-profile</t>
+    <t xml:space="preserve">physicalDomain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhysicalDomain</t>
   </si>
   <si>
     <t xml:space="preserve">immediate</t>
@@ -399,16 +378,10 @@
     <t xml:space="preserve">cnttype</t>
   </si>
   <si>
-    <t xml:space="preserve">permit-all</t>
-  </si>
-  <si>
     <t xml:space="preserve">provider</t>
   </si>
   <si>
     <t xml:space="preserve">consumer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer3</t>
   </si>
 </sst>
 </file>
@@ -424,6 +397,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -509,20 +483,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,31 +516,25 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -587,197 +553,184 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>6</v>
+        <v>101</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>103</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>106</v>
-      </c>
       <c r="H4" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>107</v>
+        <v>23</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -796,22 +749,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.54"/>
@@ -819,212 +772,177 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>105</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1043,342 +961,226 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1400,12 +1202,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.46"/>
@@ -1414,36 +1216,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1465,17 +1267,17 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.54"/>
@@ -1483,147 +1285,147 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="D2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="F2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="H4" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1645,50 +1447,50 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1710,137 +1512,137 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1859,10 +1661,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1893,286 +1695,357 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="P1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="Q1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="T1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="W1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="E2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="0" t="s">
+      <c r="S2" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="T2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="W2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="E3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="S3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="S3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="R4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="M5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="0" t="s">
+      <c r="O5" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="W4" s="0" t="s">
-        <v>11</v>
+      <c r="P5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2191,159 +2064,197 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>42</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
+      <c r="H2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>11</v>
+      <c r="H3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>11</v>
+      <c r="H6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2365,141 +2276,151 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>65535</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>65535</v>
+        <v>60</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>65535</v>
+        <v>60</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>53</v>
@@ -2507,40 +2428,46 @@
       <c r="M3" s="0" t="n">
         <v>53</v>
       </c>
+      <c r="N3" s="0" t="s">
+        <v>80</v>
+      </c>
       <c r="O3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>78</v>
+      <c r="F4" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>65535</v>
+        <v>60</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>53</v>
@@ -2548,40 +2475,46 @@
       <c r="M4" s="0" t="n">
         <v>53</v>
       </c>
+      <c r="N4" s="0" t="s">
+        <v>80</v>
+      </c>
       <c r="O4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>65535</v>
+        <v>49</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>443</v>
@@ -2589,8 +2522,11 @@
       <c r="M5" s="0" t="n">
         <v>443</v>
       </c>
+      <c r="N5" s="0" t="s">
+        <v>80</v>
+      </c>
       <c r="O5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2612,12 +2548,12 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.43"/>
@@ -2630,115 +2566,118 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>93</v>
-      </c>
       <c r="I3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>93</v>
-      </c>
       <c r="I4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>